<commit_message>
add 2018 to Terry
</commit_message>
<xml_diff>
--- a/excel/02/1420 Terry - 3 - Add Expenses.xlsx
+++ b/excel/02/1420 Terry - 3 - Add Expenses.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/github/benofben/the_intelligent_property_investor/excel/2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/github/benofben/the_intelligent_property_investor/excel/02/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C23C75-101B-E14D-B578-614FBBD5B16C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{6B2BACE4-D29B-AC4D-90BF-6B88B76DFC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -751,109 +752,109 @@
                   <c:v>0.12762033041868479</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1308764768451402</c:v>
+                  <c:v>9.7957771794393245E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.11825992501782338</c:v>
+                  <c:v>0.10180707771273019</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1089832785160367</c:v>
+                  <c:v>9.4516616521544528E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12415150577122339</c:v>
+                  <c:v>0.11120610065458818</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.11587678867069232</c:v>
+                  <c:v>0.10413355823681948</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10917469914585058</c:v>
+                  <c:v>9.8405185146436314E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.10363718987644618</c:v>
+                  <c:v>9.367221201848934E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.8986119369243036E-2</c:v>
+                  <c:v>8.969690360199524E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.5025366601148936E-2</c:v>
+                  <c:v>8.6311629817000871E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.1612672886868765E-2</c:v>
+                  <c:v>8.3394798217715047E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>8.8642338676826818E-2</c:v>
+                  <c:v>8.0856064465673894E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.603418802487961E-2</c:v>
+                  <c:v>7.8626899954152951E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8.372630282816898E-2</c:v>
+                  <c:v>7.6654381561405471E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.1670105375260607E-2</c:v>
+                  <c:v>7.489698856814031E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.9826948988292762E-2</c:v>
+                  <c:v>7.3321688584785313E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.8165703409023651E-2</c:v>
+                  <c:v>7.1901873713958731E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.6661012023533565E-2</c:v>
+                  <c:v>7.0615870952075041E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.5292012504227984E-2</c:v>
+                  <c:v>6.944584868657569E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.4041383206265118E-2</c:v>
+                  <c:v>6.8377001624502262E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.2894622489126093E-2</c:v>
+                  <c:v>6.7396934808650957E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.1839497183764367E-2</c:v>
+                  <c:v>6.649519220714728E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.0865615633398327E-2</c:v>
+                  <c:v>6.5662891779567745E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.9964093672193556E-2</c:v>
+                  <c:v>6.4892439979655894E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.9127290766296659E-2</c:v>
+                  <c:v>6.4177306227745479E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.834859970469527E-2</c:v>
+                  <c:v>6.3511843153706588E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.7273492727653081E-2</c:v>
+                  <c:v>6.2542357279826849E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.7273492727653095E-2</c:v>
+                  <c:v>6.2542357279826863E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.7273492727653081E-2</c:v>
+                  <c:v>6.2542357279826863E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.7273492727653109E-2</c:v>
+                  <c:v>6.2542357279826877E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.7273492727653053E-2</c:v>
+                  <c:v>6.2542357279826821E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.7273492727653053E-2</c:v>
+                  <c:v>6.2542357279826807E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.7273492727653039E-2</c:v>
+                  <c:v>6.2542357279826807E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.7273492727653122E-2</c:v>
+                  <c:v>6.2542357279826891E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.7273492727653067E-2</c:v>
+                  <c:v>6.2542357279826835E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.7273492727653136E-2</c:v>
+                  <c:v>6.2542357279826905E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1357,109 +1358,109 @@
                   <c:v>-8691.4900000000016</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-6597.0396000000037</c:v>
+                  <c:v>-9778.260000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-6159.5363880000059</c:v>
+                  <c:v>-8066.1492000000035</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-5708.9080796400067</c:v>
+                  <c:v>-7672.7192760000016</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-1764.2809220292038</c:v>
+                  <c:v>-3787.0064542800064</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-1286.2093496900779</c:v>
+                  <c:v>-3369.6166479084059</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-793.79563018077897</c:v>
+                  <c:v>-2939.7051473456559</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-286.60949908620387</c:v>
+                  <c:v>-2496.8963017660226</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>235.79221594120827</c:v>
+                  <c:v>-2040.8031908190078</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>773.86598241944921</c:v>
+                  <c:v>-1571.0272865435763</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1328.0819618920304</c:v>
+                  <c:v>-1087.158105139888</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1898.9244207487955</c:v>
+                  <c:v>-588.77284829407836</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2486.8921533712619</c:v>
+                  <c:v>-75.436033742897052</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3092.4989179723943</c:v>
+                  <c:v>453.30088524481107</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3716.2738855115676</c:v>
+                  <c:v>997.8999118021602</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4358.7621020769129</c:v>
+                  <c:v>1558.8369091562217</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5020.5249651392169</c:v>
+                  <c:v>2136.602016430912</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5702.1407140933916</c:v>
+                  <c:v>2731.700076923833</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6404.204935516198</c:v>
+                  <c:v>3344.6510792315494</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7127.331083581681</c:v>
+                  <c:v>3975.9906116084949</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7872.1510160891321</c:v>
+                  <c:v>4626.2703299567456</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>8639.3155465718046</c:v>
+                  <c:v>5296.0584398554493</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>9429.4950129689569</c:v>
+                  <c:v>5985.9401930511103</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10243.379863358032</c:v>
+                  <c:v>6696.5183988426434</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>11081.681259258776</c:v>
+                  <c:v>7428.4139508079279</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>11945.131697036544</c:v>
+                  <c:v>8182.2663693321665</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>30534.485647947637</c:v>
+                  <c:v>26658.734360412134</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>31450.520217386067</c:v>
+                  <c:v>27458.4963912245</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>32394.035823907649</c:v>
+                  <c:v>28282.251282961235</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>33365.856898624879</c:v>
+                  <c:v>29130.718821450078</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>34366.832605583622</c:v>
+                  <c:v>30004.640386093575</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>35397.837583751141</c:v>
+                  <c:v>30904.779597676381</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>36459.772711263671</c:v>
+                  <c:v>31831.922985606678</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>37553.565892601582</c:v>
+                  <c:v>32786.880675174878</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>38680.172869379632</c:v>
+                  <c:v>33770.48709543013</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>39840.578055461025</c:v>
+                  <c:v>34783.601708293034</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3111,7 +3112,7 @@
   <dimension ref="A1:Q71"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="D10" sqref="D2:D10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3555,19 +3556,18 @@
         <v>-290.04000000000002</v>
       </c>
       <c r="E8" s="5">
-        <f t="shared" ref="E8:E67" si="9">E7*(1+B8)</f>
-        <v>-378.12330000000009</v>
+        <f>-2234.42-C8-D8</f>
+        <v>-469.38000000000005</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" ref="F8:F34" si="10">F7*(1+B8)</f>
+        <f t="shared" ref="F8:F34" si="9">F7*(1+B8)</f>
         <v>-569.59</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" ref="G8:G39" si="11">G7*(1+B7)</f>
-        <v>2163</v>
+        <v>2100</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>-1330.14</v>
       </c>
       <c r="I8" s="10">
         <f t="shared" si="0"/>
@@ -3591,15 +3591,15 @@
       </c>
       <c r="N8" s="8">
         <f t="shared" si="6"/>
-        <v>12647.730746943227</v>
+        <v>9466.5103469432288</v>
       </c>
       <c r="O8" s="13">
         <f t="shared" si="7"/>
-        <v>0.1308764768451402</v>
+        <v>9.7957771794393245E-2</v>
       </c>
       <c r="P8" s="8">
         <f t="shared" si="5"/>
-        <v>-6597.0396000000037</v>
+        <v>-9778.260000000002</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -3618,16 +3618,16 @@
         <v>-290.04000000000002</v>
       </c>
       <c r="E9" s="5">
+        <f t="shared" ref="E8:E67" si="10">E8*(1+B9)</f>
+        <v>-483.46140000000008</v>
+      </c>
+      <c r="F9" s="5">
         <f t="shared" si="9"/>
-        <v>-389.4669990000001</v>
-      </c>
-      <c r="F9" s="5">
-        <f t="shared" si="10"/>
         <v>-586.67770000000007</v>
       </c>
       <c r="G9" s="5">
-        <f t="shared" si="11"/>
-        <v>2227.89</v>
+        <f t="shared" ref="G9:G39" si="11">G8*(1+B8)</f>
+        <v>2163</v>
       </c>
       <c r="H9" s="5">
         <v>0</v>
@@ -3654,15 +3654,15 @@
       </c>
       <c r="N9" s="8">
         <f t="shared" si="6"/>
-        <v>13704.368855069975</v>
+        <v>11797.756043069978</v>
       </c>
       <c r="O9" s="13">
         <f t="shared" si="7"/>
-        <v>0.11825992501782338</v>
+        <v>0.10180707771273019</v>
       </c>
       <c r="P9" s="8">
         <f t="shared" si="5"/>
-        <v>-6159.5363880000059</v>
+        <v>-8066.1492000000035</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3681,16 +3681,16 @@
         <v>-290.04000000000002</v>
       </c>
       <c r="E10" s="5">
+        <f t="shared" si="10"/>
+        <v>-497.9652420000001</v>
+      </c>
+      <c r="F10" s="5">
         <f t="shared" si="9"/>
-        <v>-401.15100897000013</v>
-      </c>
-      <c r="F10" s="5">
-        <f t="shared" si="10"/>
         <v>-604.27803100000006</v>
       </c>
       <c r="G10" s="5">
         <f t="shared" si="11"/>
-        <v>2294.7266999999997</v>
+        <v>2227.89</v>
       </c>
       <c r="H10" s="5">
         <v>0</v>
@@ -3717,15 +3717,15 @@
       </c>
       <c r="N10" s="8">
         <f t="shared" si="6"/>
-        <v>14794.192512916694</v>
+        <v>12830.381316556699</v>
       </c>
       <c r="O10" s="13">
         <f t="shared" si="7"/>
-        <v>0.1089832785160367</v>
+        <v>9.4516616521544528E-2</v>
       </c>
       <c r="P10" s="8">
         <f t="shared" si="5"/>
-        <v>-5708.9080796400067</v>
+        <v>-7672.7192760000016</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -3744,16 +3744,16 @@
         <v>0</v>
       </c>
       <c r="E11" s="5">
+        <f t="shared" si="10"/>
+        <v>-512.90419926000015</v>
+      </c>
+      <c r="F11" s="5">
         <f t="shared" si="9"/>
-        <v>-413.18553923910014</v>
-      </c>
-      <c r="F11" s="5">
-        <f t="shared" si="10"/>
         <v>-622.40637193000009</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="11"/>
-        <v>2363.5685009999997</v>
+        <v>2294.7266999999997</v>
       </c>
       <c r="H11" s="5">
         <v>0</v>
@@ -3780,15 +3780,15 @@
       </c>
       <c r="N11" s="8">
         <f t="shared" si="6"/>
-        <v>19398.730153924225</v>
+        <v>17376.004621673423</v>
       </c>
       <c r="O11" s="13">
         <f t="shared" si="7"/>
-        <v>0.12415150577122339</v>
+        <v>0.11120610065458818</v>
       </c>
       <c r="P11" s="8">
         <f t="shared" si="5"/>
-        <v>-1764.2809220292038</v>
+        <v>-3787.0064542800064</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
@@ -3807,16 +3807,16 @@
         <v>0</v>
       </c>
       <c r="E12" s="5">
+        <f t="shared" si="10"/>
+        <v>-528.29132523780015</v>
+      </c>
+      <c r="F12" s="5">
         <f t="shared" si="9"/>
-        <v>-425.58110541627315</v>
-      </c>
-      <c r="F12" s="5">
-        <f t="shared" si="10"/>
         <v>-641.07856308790008</v>
       </c>
       <c r="G12" s="5">
         <f t="shared" si="11"/>
-        <v>2434.47555603</v>
+        <v>2363.5685009999997</v>
       </c>
       <c r="H12" s="5">
         <v>0</v>
@@ -3843,15 +3843,15 @@
       </c>
       <c r="N12" s="8">
         <f t="shared" si="6"/>
-        <v>20558.103544852711</v>
+        <v>18474.696246634383</v>
       </c>
       <c r="O12" s="13">
         <f t="shared" si="7"/>
-        <v>0.11587678867069232</v>
+        <v>0.10413355823681948</v>
       </c>
       <c r="P12" s="8">
         <f t="shared" si="5"/>
-        <v>-1286.2093496900779</v>
+        <v>-3369.6166479084059</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
@@ -3870,16 +3870,16 @@
         <v>0</v>
       </c>
       <c r="E13" s="5">
+        <f t="shared" si="10"/>
+        <v>-544.14006499493416</v>
+      </c>
+      <c r="F13" s="5">
         <f t="shared" si="9"/>
-        <v>-438.34853857876135</v>
-      </c>
-      <c r="F13" s="5">
-        <f t="shared" si="10"/>
         <v>-660.31091998053705</v>
       </c>
       <c r="G13" s="5">
         <f t="shared" si="11"/>
-        <v>2507.5098227109002</v>
+        <v>2434.47555603</v>
       </c>
       <c r="H13" s="5">
         <v>0</v>
@@ -3906,15 +3906,15 @@
       </c>
       <c r="N13" s="8">
         <f t="shared" si="6"/>
-        <v>21753.908852658984</v>
+        <v>19607.999335494107</v>
       </c>
       <c r="O13" s="13">
         <f t="shared" si="7"/>
-        <v>0.10917469914585058</v>
+        <v>9.8405185146436314E-2</v>
       </c>
       <c r="P13" s="8">
         <f t="shared" si="5"/>
-        <v>-793.79563018077897</v>
+        <v>-2939.7051473456559</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
@@ -3933,16 +3933,16 @@
         <v>0</v>
       </c>
       <c r="E14" s="5">
+        <f t="shared" si="10"/>
+        <v>-560.46426694478225</v>
+      </c>
+      <c r="F14" s="5">
         <f t="shared" si="9"/>
-        <v>-451.49899473612419</v>
-      </c>
-      <c r="F14" s="5">
-        <f t="shared" si="10"/>
         <v>-680.12024757995323</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="11"/>
-        <v>2582.735117392227</v>
+        <v>2507.5098227109002</v>
       </c>
       <c r="H14" s="5">
         <v>0</v>
@@ -3969,15 +3969,15 @@
       </c>
       <c r="N14" s="8">
         <f t="shared" si="6"/>
-        <v>22987.297745757169</v>
+        <v>20777.010943077352</v>
       </c>
       <c r="O14" s="13">
         <f t="shared" si="7"/>
-        <v>0.10363718987644618</v>
+        <v>9.367221201848934E-2</v>
       </c>
       <c r="P14" s="8">
         <f t="shared" si="5"/>
-        <v>-286.60949908620387</v>
+        <v>-2496.8963017660226</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
@@ -3996,16 +3996,16 @@
         <v>0</v>
       </c>
       <c r="E15" s="5">
+        <f t="shared" si="10"/>
+        <v>-577.27819495312576</v>
+      </c>
+      <c r="F15" s="5">
         <f t="shared" si="9"/>
-        <v>-465.04396457820792</v>
-      </c>
-      <c r="F15" s="5">
-        <f t="shared" si="10"/>
         <v>-700.52385500735181</v>
       </c>
       <c r="G15" s="5">
         <f t="shared" si="11"/>
-        <v>2660.2171709139939</v>
+        <v>2582.735117392227</v>
       </c>
       <c r="H15" s="5">
         <v>0</v>
@@ -4032,15 +4032,15 @@
       </c>
       <c r="N15" s="8">
         <f t="shared" si="6"/>
-        <v>24259.45853078234</v>
+        <v>21982.863124022122</v>
       </c>
       <c r="O15" s="13">
         <f t="shared" si="7"/>
-        <v>9.8986119369243036E-2</v>
+        <v>8.969690360199524E-2</v>
       </c>
       <c r="P15" s="8">
         <f t="shared" si="5"/>
-        <v>235.79221594120827</v>
+        <v>-2040.8031908190078</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
@@ -4059,16 +4059,16 @@
         <v>0</v>
       </c>
       <c r="E16" s="5">
+        <f t="shared" si="10"/>
+        <v>-594.59654080171958</v>
+      </c>
+      <c r="F16" s="5">
         <f t="shared" si="9"/>
-        <v>-478.99528351555415</v>
-      </c>
-      <c r="F16" s="5">
-        <f t="shared" si="10"/>
         <v>-721.53957065757243</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="11"/>
-        <v>2740.0236860414138</v>
+        <v>2660.2171709139939</v>
       </c>
       <c r="H16" s="5">
         <v>0</v>
@@ -4095,15 +4095,15 @@
       </c>
       <c r="N16" s="8">
         <f t="shared" si="6"/>
-        <v>25571.617326006162</v>
+        <v>23226.724057043139</v>
       </c>
       <c r="O16" s="13">
         <f t="shared" si="7"/>
-        <v>9.5025366601148936E-2</v>
+        <v>8.6311629817000871E-2</v>
       </c>
       <c r="P16" s="8">
         <f t="shared" si="5"/>
-        <v>773.86598241944921</v>
+        <v>-1571.0272865435763</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.2">
@@ -4122,16 +4122,16 @@
         <v>0</v>
       </c>
       <c r="E17" s="5">
+        <f t="shared" si="10"/>
+        <v>-612.43443702577122</v>
+      </c>
+      <c r="F17" s="5">
         <f t="shared" si="9"/>
-        <v>-493.3651420210208</v>
-      </c>
-      <c r="F17" s="5">
-        <f t="shared" si="10"/>
         <v>-743.18575777729961</v>
       </c>
       <c r="G17" s="5">
         <f t="shared" si="11"/>
-        <v>2822.2243966226565</v>
+        <v>2740.0236860414138</v>
       </c>
       <c r="H17" s="5">
         <v>0</v>
@@ -4158,15 +4158,15 @@
       </c>
       <c r="N17" s="8">
         <f t="shared" si="6"/>
-        <v>26925.039272598231</v>
+        <v>24509.799205566313</v>
       </c>
       <c r="O17" s="13">
         <f t="shared" si="7"/>
-        <v>9.1612672886868765E-2</v>
+        <v>8.3394798217715047E-2</v>
       </c>
       <c r="P17" s="8">
         <f t="shared" si="5"/>
-        <v>1328.0819618920304</v>
+        <v>-1087.158105139888</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.2">
@@ -4185,16 +4185,16 @@
         <v>0</v>
       </c>
       <c r="E18" s="5">
+        <f t="shared" si="10"/>
+        <v>-630.80747013654434</v>
+      </c>
+      <c r="F18" s="5">
         <f t="shared" si="9"/>
-        <v>-508.16609628165145</v>
-      </c>
-      <c r="F18" s="5">
-        <f t="shared" si="10"/>
         <v>-765.48133051061859</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="11"/>
-        <v>2906.8911285213362</v>
+        <v>2822.2243966226565</v>
       </c>
       <c r="H18" s="5">
         <v>0</v>
@@ -4221,15 +4221,15 @@
       </c>
       <c r="N18" s="8">
         <f t="shared" si="6"/>
-        <v>28321.029784958417</v>
+        <v>25833.332515915543</v>
       </c>
       <c r="O18" s="13">
         <f t="shared" si="7"/>
-        <v>8.8642338676826818E-2</v>
+        <v>8.0856064465673894E-2</v>
       </c>
       <c r="P18" s="8">
         <f t="shared" si="5"/>
-        <v>1898.9244207487955</v>
+        <v>-588.77284829407836</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.2">
@@ -4248,16 +4248,16 @@
         <v>0</v>
       </c>
       <c r="E19" s="5">
+        <f t="shared" si="10"/>
+        <v>-649.73169424064065</v>
+      </c>
+      <c r="F19" s="5">
         <f t="shared" si="9"/>
-        <v>-523.41107917010106</v>
-      </c>
-      <c r="F19" s="5">
-        <f t="shared" si="10"/>
         <v>-788.44577042593721</v>
       </c>
       <c r="G19" s="5">
         <f t="shared" si="11"/>
-        <v>2994.0978623769765</v>
+        <v>2906.8911285213362</v>
       </c>
       <c r="H19" s="5">
         <v>0</v>
@@ -4284,15 +4284,15 @@
       </c>
       <c r="N19" s="8">
         <f t="shared" si="6"/>
-        <v>29760.93584139525</v>
+        <v>27198.607654281092</v>
       </c>
       <c r="O19" s="13">
         <f t="shared" si="7"/>
-        <v>8.603418802487961E-2</v>
+        <v>7.8626899954152951E-2</v>
       </c>
       <c r="P19" s="8">
         <f t="shared" si="5"/>
-        <v>2486.8921533712619</v>
+        <v>-75.436033742897052</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.2">
@@ -4311,16 +4311,16 @@
         <v>0</v>
       </c>
       <c r="E20" s="5">
+        <f t="shared" si="10"/>
+        <v>-669.22364506785993</v>
+      </c>
+      <c r="F20" s="5">
         <f t="shared" si="9"/>
-        <v>-539.11341154520414</v>
-      </c>
-      <c r="F20" s="5">
-        <f t="shared" si="10"/>
         <v>-812.09914353871534</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" si="11"/>
-        <v>3083.9207982482858</v>
+        <v>2994.0978623769765</v>
       </c>
       <c r="H20" s="5">
         <v>0</v>
@@ -4347,15 +4347,15 @@
       </c>
       <c r="N20" s="8">
         <f t="shared" si="6"/>
-        <v>31246.147316454109</v>
+        <v>28606.949283726528</v>
       </c>
       <c r="O20" s="13">
         <f t="shared" si="7"/>
-        <v>8.372630282816898E-2</v>
+        <v>7.6654381561405471E-2</v>
       </c>
       <c r="P20" s="8">
         <f t="shared" si="5"/>
-        <v>3092.4989179723943</v>
+        <v>453.30088524481107</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
@@ -4374,16 +4374,16 @@
         <v>0</v>
       </c>
       <c r="E21" s="5">
+        <f t="shared" si="10"/>
+        <v>-689.30035441989571</v>
+      </c>
+      <c r="F21" s="5">
         <f t="shared" si="9"/>
-        <v>-555.28681389156031</v>
-      </c>
-      <c r="F21" s="5">
-        <f t="shared" si="10"/>
         <v>-836.46211784487684</v>
       </c>
       <c r="G21" s="5">
         <f t="shared" si="11"/>
-        <v>3176.4384221957343</v>
+        <v>3083.9207982482858</v>
       </c>
       <c r="H21" s="5">
         <v>0</v>
@@ -4410,15 +4410,15 @@
       </c>
       <c r="N21" s="8">
         <f t="shared" si="6"/>
-        <v>32778.098356257957</v>
+        <v>30059.724382548549</v>
       </c>
       <c r="O21" s="13">
         <f t="shared" si="7"/>
-        <v>8.1670105375260607E-2</v>
+        <v>7.489698856814031E-2</v>
       </c>
       <c r="P21" s="8">
         <f t="shared" si="5"/>
-        <v>3716.2738855115676</v>
+        <v>997.8999118021602</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.2">
@@ -4437,16 +4437,16 @@
         <v>0</v>
       </c>
       <c r="E22" s="5">
+        <f t="shared" si="10"/>
+        <v>-709.97936505249265</v>
+      </c>
+      <c r="F22" s="5">
         <f t="shared" si="9"/>
-        <v>-571.94541830830713</v>
-      </c>
-      <c r="F22" s="5">
-        <f t="shared" si="10"/>
         <v>-861.55598138022322</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="11"/>
-        <v>3271.7315748616065</v>
+        <v>3176.4384221957343</v>
       </c>
       <c r="H22" s="5">
         <v>0</v>
@@ -4473,15 +4473,15 @@
       </c>
       <c r="N22" s="8">
         <f t="shared" si="6"/>
-        <v>34358.268798249206</v>
+        <v>31558.343605328511</v>
       </c>
       <c r="O22" s="13">
         <f t="shared" si="7"/>
-        <v>7.9826948988292762E-2</v>
+        <v>7.3321688584785313E-2</v>
       </c>
       <c r="P22" s="8">
         <f t="shared" si="5"/>
-        <v>4358.7621020769129</v>
+        <v>1558.8369091562217</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.2">
@@ -4500,16 +4500,16 @@
         <v>0</v>
       </c>
       <c r="E23" s="5">
+        <f t="shared" si="10"/>
+        <v>-731.27874600406744</v>
+      </c>
+      <c r="F23" s="5">
         <f t="shared" si="9"/>
-        <v>-589.10378085755633</v>
-      </c>
-      <c r="F23" s="5">
-        <f t="shared" si="10"/>
         <v>-887.40266082162998</v>
       </c>
       <c r="G23" s="5">
         <f t="shared" si="11"/>
-        <v>3369.8835221074546</v>
+        <v>3271.7315748616065</v>
       </c>
       <c r="H23" s="5">
         <v>0</v>
@@ -4536,15 +4536,15 @@
       </c>
       <c r="N23" s="8">
         <f t="shared" si="6"/>
-        <v>35988.185636786155</v>
+        <v>33104.262688077855</v>
       </c>
       <c r="O23" s="13">
         <f t="shared" si="7"/>
-        <v>7.8165703409023651E-2</v>
+        <v>7.1901873713958731E-2</v>
       </c>
       <c r="P23" s="8">
         <f t="shared" si="5"/>
-        <v>5020.5249651392169</v>
+        <v>2136.602016430912</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.2">
@@ -4563,16 +4563,16 @@
         <v>0</v>
       </c>
       <c r="E24" s="5">
+        <f t="shared" si="10"/>
+        <v>-753.21710838418949</v>
+      </c>
+      <c r="F24" s="5">
         <f t="shared" si="9"/>
-        <v>-606.77689428328301</v>
-      </c>
-      <c r="F24" s="5">
-        <f t="shared" si="10"/>
         <v>-914.02474064627893</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="11"/>
-        <v>3470.9800277706781</v>
+        <v>3369.8835221074546</v>
       </c>
       <c r="H24" s="5">
         <v>0</v>
@@ -4599,15 +4599,15 @@
       </c>
       <c r="N24" s="8">
         <f t="shared" si="6"/>
-        <v>37669.424536077175</v>
+        <v>34698.983898907623</v>
       </c>
       <c r="O24" s="13">
         <f t="shared" si="7"/>
-        <v>7.6661012023533565E-2</v>
+        <v>7.0615870952075041E-2</v>
       </c>
       <c r="P24" s="8">
         <f t="shared" si="5"/>
-        <v>5702.1407140933916</v>
+        <v>2731.700076923833</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.2">
@@ -4626,16 +4626,16 @@
         <v>0</v>
       </c>
       <c r="E25" s="5">
+        <f t="shared" si="10"/>
+        <v>-775.81362163571521</v>
+      </c>
+      <c r="F25" s="5">
         <f t="shared" si="9"/>
-        <v>-624.98020111178153</v>
-      </c>
-      <c r="F25" s="5">
-        <f t="shared" si="10"/>
         <v>-941.44548286566737</v>
       </c>
       <c r="G25" s="5">
         <f t="shared" si="11"/>
-        <v>3575.1094286037987</v>
+        <v>3470.9800277706781</v>
       </c>
       <c r="H25" s="5">
         <v>0</v>
@@ -4662,15 +4662,15 @@
       </c>
       <c r="N25" s="8">
         <f t="shared" si="6"/>
-        <v>39403.611392000137</v>
+        <v>36344.057535715488</v>
       </c>
       <c r="O25" s="13">
         <f t="shared" si="7"/>
-        <v>7.5292012504227984E-2</v>
+        <v>6.944584868657569E-2</v>
       </c>
       <c r="P25" s="8">
         <f t="shared" si="5"/>
-        <v>6404.204935516198</v>
+        <v>3344.6510792315494</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.2">
@@ -4689,16 +4689,16 @@
         <v>0</v>
       </c>
       <c r="E26" s="5">
+        <f t="shared" si="10"/>
+        <v>-799.08803028478667</v>
+      </c>
+      <c r="F26" s="5">
         <f t="shared" si="9"/>
-        <v>-643.72960714513499</v>
-      </c>
-      <c r="F26" s="5">
-        <f t="shared" si="10"/>
         <v>-969.68884735163738</v>
       </c>
       <c r="G26" s="5">
         <f t="shared" si="11"/>
-        <v>3682.3627114619126</v>
+        <v>3575.1094286037987</v>
       </c>
       <c r="H26" s="5">
         <v>0</v>
@@ -4725,15 +4725,15 @@
       </c>
       <c r="N26" s="8">
         <f t="shared" si="6"/>
-        <v>41192.423944391558</v>
+        <v>38041.083472418373</v>
       </c>
       <c r="O26" s="13">
         <f t="shared" si="7"/>
-        <v>7.4041383206265118E-2</v>
+        <v>6.8377001624502262E-2</v>
       </c>
       <c r="P26" s="8">
         <f t="shared" si="5"/>
-        <v>7127.331083581681</v>
+        <v>3975.9906116084949</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.2">
@@ -4752,16 +4752,16 @@
         <v>0</v>
       </c>
       <c r="E27" s="5">
+        <f t="shared" si="10"/>
+        <v>-823.06067119333034</v>
+      </c>
+      <c r="F27" s="5">
         <f t="shared" si="9"/>
-        <v>-663.04149535948909</v>
-      </c>
-      <c r="F27" s="5">
-        <f t="shared" si="10"/>
         <v>-998.77951277218654</v>
       </c>
       <c r="G27" s="5">
         <f t="shared" si="11"/>
-        <v>3792.83359280577</v>
+        <v>3682.3627114619126</v>
       </c>
       <c r="H27" s="5">
         <v>0</v>
@@ -4788,15 +4788,15 @@
       </c>
       <c r="N27" s="8">
         <f t="shared" si="6"/>
-        <v>43037.593441451667</v>
+        <v>39791.712755319277</v>
       </c>
       <c r="O27" s="13">
         <f t="shared" si="7"/>
-        <v>7.2894622489126093E-2</v>
+        <v>6.7396934808650957E-2</v>
       </c>
       <c r="P27" s="8">
         <f t="shared" si="5"/>
-        <v>7872.1510160891321</v>
+        <v>4626.2703299567456</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.2">
@@ -4815,16 +4815,16 @@
         <v>0</v>
       </c>
       <c r="E28" s="5">
+        <f t="shared" si="10"/>
+        <v>-847.75249132913029</v>
+      </c>
+      <c r="F28" s="5">
         <f t="shared" si="9"/>
-        <v>-682.93274022027379</v>
-      </c>
-      <c r="F28" s="5">
-        <f t="shared" si="10"/>
         <v>-1028.7428981553521</v>
       </c>
       <c r="G28" s="5">
         <f t="shared" si="11"/>
-        <v>3906.6186005899431</v>
+        <v>3792.83359280577</v>
       </c>
       <c r="H28" s="5">
         <v>0</v>
@@ -4851,15 +4851,15 @@
       </c>
       <c r="N28" s="8">
         <f t="shared" si="6"/>
-        <v>44940.906357963977</v>
+        <v>41597.649251247625</v>
       </c>
       <c r="O28" s="13">
         <f t="shared" si="7"/>
-        <v>7.1839497183764367E-2</v>
+        <v>6.649519220714728E-2</v>
       </c>
       <c r="P28" s="8">
         <f t="shared" si="5"/>
-        <v>8639.3155465718046</v>
+        <v>5296.0584398554493</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.2">
@@ -4878,16 +4878,16 @@
         <v>0</v>
       </c>
       <c r="E29" s="5">
+        <f t="shared" si="10"/>
+        <v>-873.18506606900428</v>
+      </c>
+      <c r="F29" s="5">
         <f t="shared" si="9"/>
-        <v>-703.42072242688198</v>
-      </c>
-      <c r="F29" s="5">
-        <f t="shared" si="10"/>
         <v>-1059.6051851000127</v>
       </c>
       <c r="G29" s="5">
         <f t="shared" si="11"/>
-        <v>4023.8171586076414</v>
+        <v>3906.6186005899431</v>
       </c>
       <c r="H29" s="5">
         <v>0</v>
@@ -4914,15 +4914,15 @@
       </c>
       <c r="N29" s="8">
         <f t="shared" si="6"/>
-        <v>46904.206169075042</v>
+        <v>43460.651349157197</v>
       </c>
       <c r="O29" s="13">
         <f t="shared" si="7"/>
-        <v>7.0865615633398327E-2</v>
+        <v>6.5662891779567745E-2</v>
       </c>
       <c r="P29" s="8">
         <f t="shared" si="5"/>
-        <v>9429.4950129689569</v>
+        <v>5985.9401930511103</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.2">
@@ -4941,16 +4941,16 @@
         <v>0</v>
       </c>
       <c r="E30" s="5">
+        <f t="shared" si="10"/>
+        <v>-899.38061805107441</v>
+      </c>
+      <c r="F30" s="5">
         <f t="shared" si="9"/>
-        <v>-724.52334409968842</v>
-      </c>
-      <c r="F30" s="5">
-        <f t="shared" si="10"/>
         <v>-1091.3933406530132</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="11"/>
-        <v>4144.531673365871</v>
+        <v>4023.8171586076414</v>
       </c>
       <c r="H30" s="5">
         <v>0</v>
@@ -4977,15 +4977,15 @@
       </c>
       <c r="N30" s="8">
         <f t="shared" si="6"/>
-        <v>48929.395181452433</v>
+        <v>45382.533716937047</v>
       </c>
       <c r="O30" s="13">
         <f t="shared" si="7"/>
-        <v>6.9964093672193556E-2</v>
+        <v>6.4892439979655894E-2</v>
       </c>
       <c r="P30" s="8">
         <f t="shared" si="5"/>
-        <v>10243.379863358032</v>
+        <v>6696.5183988426434</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.2">
@@ -5004,16 +5004,16 @@
         <v>0</v>
       </c>
       <c r="E31" s="5">
+        <f t="shared" si="10"/>
+        <v>-926.36203659260661</v>
+      </c>
+      <c r="F31" s="5">
         <f t="shared" si="9"/>
-        <v>-746.25904442267904</v>
-      </c>
-      <c r="F31" s="5">
-        <f t="shared" si="10"/>
         <v>-1124.1351408726036</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" si="11"/>
-        <v>4268.8676235668472</v>
+        <v>4144.531673365871</v>
       </c>
       <c r="H31" s="5">
         <v>0</v>
@@ -5040,15 +5040,15 @@
       </c>
       <c r="N31" s="8">
         <f t="shared" si="6"/>
-        <v>51018.436423683081</v>
+        <v>47365.169115232231</v>
       </c>
       <c r="O31" s="13">
         <f t="shared" si="7"/>
-        <v>6.9127290766296659E-2</v>
+        <v>6.4177306227745479E-2</v>
       </c>
       <c r="P31" s="8">
         <f t="shared" si="5"/>
-        <v>11081.681259258776</v>
+        <v>7428.4139508079279</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.2">
@@ -5067,16 +5067,16 @@
         <v>0</v>
       </c>
       <c r="E32" s="5">
+        <f t="shared" si="10"/>
+        <v>-954.15289769038486</v>
+      </c>
+      <c r="F32" s="5">
         <f t="shared" si="9"/>
-        <v>-768.6468157553594</v>
-      </c>
-      <c r="F32" s="5">
-        <f t="shared" si="10"/>
         <v>-1157.8591950987818</v>
       </c>
       <c r="G32" s="5">
         <f t="shared" si="11"/>
-        <v>4396.9336522738531</v>
+        <v>4268.8676235668472</v>
       </c>
       <c r="H32" s="5">
         <v>0</v>
@@ -5103,15 +5103,15 @@
       </c>
       <c r="N32" s="8">
         <f t="shared" si="6"/>
-        <v>53173.355597848291</v>
+        <v>49410.490270143913</v>
       </c>
       <c r="O32" s="13">
         <f t="shared" si="7"/>
-        <v>6.834859970469527E-2</v>
+        <v>6.3511843153706588E-2</v>
       </c>
       <c r="P32" s="8">
         <f t="shared" si="5"/>
-        <v>11945.131697036544</v>
+        <v>8182.2663693321665</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.2">
@@ -5129,16 +5129,16 @@
         <v>0</v>
       </c>
       <c r="E33" s="5">
+        <f t="shared" si="10"/>
+        <v>-982.77748462109639</v>
+      </c>
+      <c r="F33" s="5">
         <f t="shared" si="9"/>
-        <v>-791.70622022802024</v>
-      </c>
-      <c r="F33" s="5">
-        <f t="shared" si="10"/>
         <v>-1192.5949709517454</v>
       </c>
       <c r="G33" s="5">
         <f t="shared" si="11"/>
-        <v>4528.8416618420688</v>
+        <v>4396.9336522738531</v>
       </c>
       <c r="H33" s="5">
         <v>0</v>
@@ -5156,15 +5156,15 @@
       </c>
       <c r="N33" s="8">
         <f t="shared" si="6"/>
-        <v>55110.518168742994</v>
+        <v>51234.766881207492</v>
       </c>
       <c r="O33" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653081E-2</v>
+        <v>6.2542357279826849E-2</v>
       </c>
       <c r="P33" s="8">
         <f t="shared" si="5"/>
-        <v>30534.485647947637</v>
+        <v>26658.734360412134</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.2">
@@ -5182,16 +5182,16 @@
         <v>0</v>
       </c>
       <c r="E34" s="5">
+        <f t="shared" si="10"/>
+        <v>-1012.2608091597293</v>
+      </c>
+      <c r="F34" s="5">
         <f t="shared" si="9"/>
-        <v>-815.45740683486088</v>
-      </c>
-      <c r="F34" s="5">
-        <f t="shared" si="10"/>
         <v>-1228.3728200802977</v>
       </c>
       <c r="G34" s="5">
         <f t="shared" si="11"/>
-        <v>4664.7069116973307</v>
+        <v>4528.8416618420688</v>
       </c>
       <c r="H34" s="5">
         <v>0</v>
@@ -5209,15 +5209,15 @@
       </c>
       <c r="N34" s="8">
         <f t="shared" si="6"/>
-        <v>56763.833713805296</v>
+        <v>52771.809887643729</v>
       </c>
       <c r="O34" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653095E-2</v>
+        <v>6.2542357279826863E-2</v>
       </c>
       <c r="P34" s="8">
         <f t="shared" si="5"/>
-        <v>31450.520217386067</v>
+        <v>27458.4963912245</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.2">
@@ -5235,8 +5235,8 @@
         <v>0</v>
       </c>
       <c r="E35" s="5">
-        <f t="shared" si="9"/>
-        <v>-839.92112903990676</v>
+        <f t="shared" si="10"/>
+        <v>-1042.6286334345211</v>
       </c>
       <c r="F35" s="5">
         <f t="shared" ref="F35:F71" si="12">F34*(1+B35)</f>
@@ -5244,7 +5244,7 @@
       </c>
       <c r="G35" s="5">
         <f t="shared" si="11"/>
-        <v>4804.6481190482509</v>
+        <v>4664.7069116973307</v>
       </c>
       <c r="H35" s="5">
         <v>0</v>
@@ -5262,15 +5262,15 @@
       </c>
       <c r="N35" s="8">
         <f t="shared" si="6"/>
-        <v>58466.748725219455</v>
+        <v>54354.964184273049</v>
       </c>
       <c r="O35" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653081E-2</v>
+        <v>6.2542357279826863E-2</v>
       </c>
       <c r="P35" s="8">
         <f t="shared" si="5"/>
-        <v>32394.035823907649</v>
+        <v>28282.251282961235</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.2">
@@ -5288,8 +5288,8 @@
         <v>0</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="9"/>
-        <v>-865.118762911104</v>
+        <f t="shared" si="10"/>
+        <v>-1073.9074924375568</v>
       </c>
       <c r="F36" s="5">
         <f t="shared" si="12"/>
@@ -5297,7 +5297,7 @@
       </c>
       <c r="G36" s="5">
         <f t="shared" si="11"/>
-        <v>4948.7875626196983</v>
+        <v>4804.6481190482509</v>
       </c>
       <c r="H36" s="5">
         <v>0</v>
@@ -5315,15 +5315,15 @@
       </c>
       <c r="N36" s="8">
         <f t="shared" si="6"/>
-        <v>60220.751186976056</v>
+        <v>55985.613109801256</v>
       </c>
       <c r="O36" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653109E-2</v>
+        <v>6.2542357279826877E-2</v>
       </c>
       <c r="P36" s="8">
         <f t="shared" si="5"/>
-        <v>33365.856898624879</v>
+        <v>29130.718821450078</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.2">
@@ -5341,8 +5341,8 @@
         <v>0</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="9"/>
-        <v>-891.07232579843719</v>
+        <f t="shared" si="10"/>
+        <v>-1106.1247172106835</v>
       </c>
       <c r="F37" s="5">
         <f t="shared" si="12"/>
@@ -5350,7 +5350,7 @@
       </c>
       <c r="G37" s="5">
         <f t="shared" si="11"/>
-        <v>5097.251189498289</v>
+        <v>4948.7875626196983</v>
       </c>
       <c r="H37" s="5">
         <v>0</v>
@@ -5368,15 +5368,15 @@
       </c>
       <c r="N37" s="8">
         <f t="shared" si="6"/>
-        <v>62027.373722585296</v>
+        <v>57665.181503095249</v>
       </c>
       <c r="O37" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653053E-2</v>
+        <v>6.2542357279826821E-2</v>
       </c>
       <c r="P37" s="8">
         <f t="shared" si="5"/>
-        <v>34366.832605583622</v>
+        <v>30004.640386093575</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.2">
@@ -5394,8 +5394,8 @@
         <v>0</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="9"/>
-        <v>-917.80449557239035</v>
+        <f t="shared" si="10"/>
+        <v>-1139.3084587270039</v>
       </c>
       <c r="F38" s="5">
         <f t="shared" si="12"/>
@@ -5403,7 +5403,7 @@
       </c>
       <c r="G38" s="5">
         <f t="shared" si="11"/>
-        <v>5250.1687251832382</v>
+        <v>5097.251189498289</v>
       </c>
       <c r="H38" s="5">
         <v>0</v>
@@ -5421,15 +5421,15 @@
       </c>
       <c r="N38" s="8">
         <f t="shared" si="6"/>
-        <v>63888.19493426285</v>
+        <v>59395.13694818809</v>
       </c>
       <c r="O38" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653053E-2</v>
+        <v>6.2542357279826807E-2</v>
       </c>
       <c r="P38" s="8">
         <f t="shared" si="5"/>
-        <v>35397.837583751141</v>
+        <v>30904.779597676381</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.2">
@@ -5447,8 +5447,8 @@
         <v>0</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="9"/>
-        <v>-945.33863043956205</v>
+        <f t="shared" si="10"/>
+        <v>-1173.4877124888139</v>
       </c>
       <c r="F39" s="5">
         <f t="shared" si="12"/>
@@ -5456,7 +5456,7 @@
       </c>
       <c r="G39" s="5">
         <f t="shared" si="11"/>
-        <v>5407.6737869387352</v>
+        <v>5250.1687251832382</v>
       </c>
       <c r="H39" s="5">
         <v>0</v>
@@ -5474,15 +5474,15 @@
       </c>
       <c r="N39" s="8">
         <f t="shared" si="6"/>
-        <v>65804.840782290732</v>
+        <v>61176.991056633735</v>
       </c>
       <c r="O39" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653039E-2</v>
+        <v>6.2542357279826807E-2</v>
       </c>
       <c r="P39" s="8">
         <f t="shared" si="5"/>
-        <v>36459.772711263671</v>
+        <v>31831.922985606678</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.2">
@@ -5500,8 +5500,8 @@
         <v>0</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="9"/>
-        <v>-973.69878935274892</v>
+        <f t="shared" si="10"/>
+        <v>-1208.6923438634783</v>
       </c>
       <c r="F40" s="5">
         <f t="shared" si="12"/>
@@ -5509,7 +5509,7 @@
       </c>
       <c r="G40" s="5">
         <f t="shared" ref="G40:G71" si="14">G39*(1+B39)</f>
-        <v>5569.9040005468978</v>
+        <v>5407.6737869387352</v>
       </c>
       <c r="H40" s="5">
         <v>0</v>
@@ -5527,15 +5527,15 @@
       </c>
       <c r="N40" s="8">
         <f t="shared" si="6"/>
-        <v>67778.986005759536</v>
+        <v>63012.300788332825</v>
       </c>
       <c r="O40" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653122E-2</v>
+        <v>6.2542357279826891E-2</v>
       </c>
       <c r="P40" s="8">
         <f t="shared" si="5"/>
-        <v>37553.565892601582</v>
+        <v>32786.880675174878</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.2">
@@ -5553,8 +5553,8 @@
         <v>0</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="9"/>
-        <v>-1002.9097530333314</v>
+        <f t="shared" si="10"/>
+        <v>-1244.9531141793827</v>
       </c>
       <c r="F41" s="5">
         <f t="shared" si="12"/>
@@ -5562,7 +5562,7 @@
       </c>
       <c r="G41" s="5">
         <f t="shared" si="14"/>
-        <v>5737.0011205633045</v>
+        <v>5569.9040005468978</v>
       </c>
       <c r="H41" s="5">
         <v>0</v>
@@ -5580,15 +5580,15 @@
       </c>
       <c r="N41" s="8">
         <f t="shared" si="6"/>
-        <v>69812.355585932266</v>
+        <v>64902.669811982763</v>
       </c>
       <c r="O41" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653067E-2</v>
+        <v>6.2542357279826835E-2</v>
       </c>
       <c r="P41" s="8">
         <f t="shared" si="5"/>
-        <v>38680.172869379632</v>
+        <v>33770.48709543013</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.2">
@@ -5606,8 +5606,8 @@
         <v>0</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="9"/>
-        <v>-1032.9970456243313</v>
+        <f t="shared" si="10"/>
+        <v>-1282.3017076047643</v>
       </c>
       <c r="F42" s="5">
         <f t="shared" si="12"/>
@@ -5615,7 +5615,7 @@
       </c>
       <c r="G42" s="5">
         <f t="shared" si="14"/>
-        <v>5909.1111541802038</v>
+        <v>5737.0011205633045</v>
       </c>
       <c r="H42" s="5">
         <v>0</v>
@@ -5633,15 +5633,15 @@
       </c>
       <c r="N42" s="8">
         <f t="shared" si="6"/>
-        <v>71906.726253510307</v>
+        <v>66849.749906342317</v>
       </c>
       <c r="O42" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653136E-2</v>
+        <v>6.2542357279826905E-2</v>
       </c>
       <c r="P42" s="8">
         <f t="shared" si="5"/>
-        <v>39840.578055461025</v>
+        <v>34783.601708293034</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.2">
@@ -5659,8 +5659,8 @@
         <v>0</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="9"/>
-        <v>-1063.9869569930613</v>
+        <f t="shared" si="10"/>
+        <v>-1320.7707588329072</v>
       </c>
       <c r="F43" s="5">
         <f t="shared" si="12"/>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="G43" s="5">
         <f t="shared" si="14"/>
-        <v>6086.3844888056101</v>
+        <v>5909.1111541802038</v>
       </c>
       <c r="H43" s="5">
         <v>0</v>
@@ -5686,15 +5686,15 @@
       </c>
       <c r="N43" s="8">
         <f t="shared" si="6"/>
-        <v>74063.928041115534</v>
+        <v>68855.242403532509</v>
       </c>
       <c r="O43" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653053E-2</v>
+        <v>6.2542357279826821E-2</v>
       </c>
       <c r="P43" s="8">
         <f t="shared" si="5"/>
-        <v>41035.79539712485</v>
+        <v>35827.109759541825</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.2">
@@ -5712,8 +5712,8 @@
         <v>0</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="9"/>
-        <v>-1095.9065657028532</v>
+        <f t="shared" si="10"/>
+        <v>-1360.3938815978945</v>
       </c>
       <c r="F44" s="5">
         <f t="shared" si="12"/>
@@ -5721,7 +5721,7 @@
       </c>
       <c r="G44" s="5">
         <f t="shared" si="14"/>
-        <v>6268.9760234697787</v>
+        <v>6086.3844888056101</v>
       </c>
       <c r="H44" s="5">
         <v>0</v>
@@ -5739,15 +5739,15 @@
       </c>
       <c r="N44" s="8">
         <f t="shared" si="6"/>
-        <v>76285.84588234908</v>
+        <v>70920.89967563856</v>
       </c>
       <c r="O44" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653122E-2</v>
+        <v>6.2542357279826891E-2</v>
       </c>
       <c r="P44" s="8">
         <f t="shared" si="5"/>
-        <v>42266.869259038605</v>
+        <v>36901.923052328086</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.2">
@@ -5765,8 +5765,8 @@
         <v>0</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="9"/>
-        <v>-1128.7837626739388</v>
+        <f t="shared" si="10"/>
+        <v>-1401.2056980458315</v>
       </c>
       <c r="F45" s="5">
         <f t="shared" si="12"/>
@@ -5774,7 +5774,7 @@
       </c>
       <c r="G45" s="5">
         <f t="shared" si="14"/>
-        <v>6457.045304173872</v>
+        <v>6268.9760234697787</v>
       </c>
       <c r="H45" s="5">
         <v>0</v>
@@ -5792,15 +5792,15 @@
       </c>
       <c r="N45" s="8">
         <f t="shared" si="6"/>
-        <v>78574.421258819493</v>
+        <v>73048.526665907673</v>
       </c>
       <c r="O45" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653067E-2</v>
+        <v>6.2542357279826849E-2</v>
       </c>
       <c r="P45" s="8">
         <f t="shared" si="5"/>
-        <v>43534.87533680976</v>
+        <v>38008.980743897926</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.2">
@@ -5818,8 +5818,8 @@
         <v>0</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="9"/>
-        <v>-1162.647275554157</v>
+        <f t="shared" si="10"/>
+        <v>-1443.2418689872065</v>
       </c>
       <c r="F46" s="5">
         <f t="shared" si="12"/>
@@ -5827,7 +5827,7 @@
       </c>
       <c r="G46" s="5">
         <f t="shared" si="14"/>
-        <v>6650.7566632990884</v>
+        <v>6457.045304173872</v>
       </c>
       <c r="H46" s="5">
         <v>0</v>
@@ -5845,15 +5845,15 @@
       </c>
       <c r="N46" s="8">
         <f t="shared" si="6"/>
-        <v>80931.653896584161</v>
+        <v>75239.982465884968</v>
       </c>
       <c r="O46" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653122E-2</v>
+        <v>6.2542357279826905E-2</v>
       </c>
       <c r="P46" s="8">
         <f t="shared" si="5"/>
-        <v>44840.92159691405</v>
+        <v>39149.250166214864</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.2">
@@ -5871,8 +5871,8 @@
         <v>0</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="9"/>
-        <v>-1197.5266938207817</v>
+        <f t="shared" si="10"/>
+        <v>-1486.5391250568227</v>
       </c>
       <c r="F47" s="5">
         <f t="shared" si="12"/>
@@ -5880,7 +5880,7 @@
       </c>
       <c r="G47" s="5">
         <f t="shared" si="14"/>
-        <v>6850.2793631980612</v>
+        <v>6650.7566632990884</v>
       </c>
       <c r="H47" s="5">
         <v>0</v>
@@ -5898,15 +5898,15 @@
       </c>
       <c r="N47" s="8">
         <f t="shared" si="6"/>
-        <v>83359.603513481648</v>
+        <v>77497.181939861475</v>
       </c>
       <c r="O47" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653095E-2</v>
+        <v>6.2542357279826863E-2</v>
       </c>
       <c r="P47" s="8">
         <f t="shared" si="5"/>
-        <v>46186.149244821478</v>
+        <v>40323.727671201312</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.2">
@@ -5924,8 +5924,8 @@
         <v>0</v>
       </c>
       <c r="E48" s="5">
-        <f t="shared" si="9"/>
-        <v>-1233.4524946354052</v>
+        <f t="shared" si="10"/>
+        <v>-1531.1352988085275</v>
       </c>
       <c r="F48" s="5">
         <f t="shared" si="12"/>
@@ -5933,7 +5933,7 @@
       </c>
       <c r="G48" s="5">
         <f t="shared" si="14"/>
-        <v>7055.7877440940028</v>
+        <v>6850.2793631980612</v>
       </c>
       <c r="H48" s="5">
         <v>0</v>
@@ -5951,15 +5951,15 @@
       </c>
       <c r="N48" s="8">
         <f t="shared" si="6"/>
-        <v>85860.391618885988</v>
+        <v>79822.097398057231</v>
       </c>
       <c r="O48" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727652998E-2</v>
+        <v>6.254235727982678E-2</v>
       </c>
       <c r="P48" s="8">
         <f t="shared" si="5"/>
-        <v>47571.733722166115</v>
+        <v>41533.439501337351</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
@@ -5977,8 +5977,8 @@
         <v>0</v>
       </c>
       <c r="E49" s="5">
-        <f t="shared" si="9"/>
-        <v>-1270.4560694744673</v>
+        <f t="shared" si="10"/>
+        <v>-1577.0693577727834</v>
       </c>
       <c r="F49" s="5">
         <f t="shared" si="12"/>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="G49" s="5">
         <f t="shared" si="14"/>
-        <v>7267.4613764168234</v>
+        <v>7055.7877440940028</v>
       </c>
       <c r="H49" s="5">
         <v>0</v>
@@ -6004,15 +6004,15 @@
       </c>
       <c r="N49" s="8">
         <f t="shared" si="6"/>
-        <v>88436.203367452734</v>
+        <v>82216.760319999099</v>
       </c>
       <c r="O49" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653136E-2</v>
+        <v>6.2542357279826905E-2</v>
       </c>
       <c r="P49" s="8">
         <f t="shared" si="5"/>
-        <v>48998.885733831106</v>
+        <v>42779.442686377472</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
@@ -6030,8 +6030,8 @@
         <v>0</v>
       </c>
       <c r="E50" s="5">
-        <f t="shared" si="9"/>
-        <v>-1308.5697515587015</v>
+        <f t="shared" si="10"/>
+        <v>-1624.381438505967</v>
       </c>
       <c r="F50" s="5">
         <f t="shared" si="12"/>
@@ -6039,7 +6039,7 @@
       </c>
       <c r="G50" s="5">
         <f t="shared" si="14"/>
-        <v>7485.485217709328</v>
+        <v>7267.4613764168234</v>
       </c>
       <c r="H50" s="5">
         <v>0</v>
@@ -6057,15 +6057,15 @@
       </c>
       <c r="N50" s="8">
         <f t="shared" si="6"/>
-        <v>91089.289468476287</v>
+        <v>84683.263129599043</v>
       </c>
       <c r="O50" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653109E-2</v>
+        <v>6.2542357279826877E-2</v>
       </c>
       <c r="P50" s="8">
         <f t="shared" si="5"/>
-        <v>50468.852305846034</v>
+        <v>44062.82596696879</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
@@ -6083,8 +6083,8 @@
         <v>0</v>
       </c>
       <c r="E51" s="5">
-        <f t="shared" si="9"/>
-        <v>-1347.8268441054624</v>
+        <f t="shared" si="10"/>
+        <v>-1673.112881661146</v>
       </c>
       <c r="F51" s="5">
         <f t="shared" si="12"/>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="G51" s="5">
         <f t="shared" si="14"/>
-        <v>7710.0497742406078</v>
+        <v>7485.485217709328</v>
       </c>
       <c r="H51" s="5">
         <v>0</v>
@@ -6110,15 +6110,15 @@
       </c>
       <c r="N51" s="8">
         <f t="shared" si="6"/>
-        <v>93821.968152530433</v>
+        <v>87223.761023486877</v>
       </c>
       <c r="O51" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727652998E-2</v>
+        <v>6.2542357279826766E-2</v>
       </c>
       <c r="P51" s="8">
         <f t="shared" si="5"/>
-        <v>51982.917875021412</v>
+        <v>45384.710745977856</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
@@ -6136,8 +6136,8 @@
         <v>0</v>
       </c>
       <c r="E52" s="5">
-        <f t="shared" si="9"/>
-        <v>-1388.2616494286262</v>
+        <f t="shared" si="10"/>
+        <v>-1723.3062681109805</v>
       </c>
       <c r="F52" s="5">
         <f t="shared" si="12"/>
@@ -6145,7 +6145,7 @@
       </c>
       <c r="G52" s="5">
         <f t="shared" si="14"/>
-        <v>7941.3512674678259</v>
+        <v>7710.0497742406078</v>
       </c>
       <c r="H52" s="5">
         <v>0</v>
@@ -6163,15 +6163,15 @@
       </c>
       <c r="N52" s="8">
         <f t="shared" si="6"/>
-        <v>96636.627197106354</v>
+        <v>89840.473854191485</v>
       </c>
       <c r="O52" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727652998E-2</v>
+        <v>6.2542357279826766E-2</v>
       </c>
       <c r="P52" s="8">
         <f t="shared" si="5"/>
-        <v>53542.405411272062</v>
+        <v>46746.252068357193</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
@@ -6189,8 +6189,8 @@
         <v>0</v>
       </c>
       <c r="E53" s="5">
-        <f t="shared" si="9"/>
-        <v>-1429.9094989114851</v>
+        <f t="shared" si="10"/>
+        <v>-1775.00545615431</v>
       </c>
       <c r="F53" s="5">
         <f t="shared" si="12"/>
@@ -6198,7 +6198,7 @@
       </c>
       <c r="G53" s="5">
         <f t="shared" si="14"/>
-        <v>8179.5918054918611</v>
+        <v>7941.3512674678259</v>
       </c>
       <c r="H53" s="5">
         <v>0</v>
@@ -6216,15 +6216,15 @@
       </c>
       <c r="N53" s="8">
         <f t="shared" si="6"/>
-        <v>99535.726013019579</v>
+        <v>92535.688069817246</v>
       </c>
       <c r="O53" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653025E-2</v>
+        <v>6.254235727982678E-2</v>
       </c>
       <c r="P53" s="8">
         <f t="shared" si="5"/>
-        <v>55148.677573610228</v>
+        <v>48148.639630407895</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
@@ -6242,8 +6242,8 @@
         <v>0</v>
       </c>
       <c r="E54" s="5">
-        <f t="shared" si="9"/>
-        <v>-1472.8067838788297</v>
+        <f t="shared" si="10"/>
+        <v>-1828.2556198389393</v>
       </c>
       <c r="F54" s="5">
         <f t="shared" si="12"/>
@@ -6251,7 +6251,7 @@
       </c>
       <c r="G54" s="5">
         <f t="shared" si="14"/>
-        <v>8424.9795596566164</v>
+        <v>8179.5918054918611</v>
       </c>
       <c r="H54" s="5">
         <v>0</v>
@@ -6269,15 +6269,15 @@
       </c>
       <c r="N54" s="8">
         <f t="shared" si="6"/>
-        <v>102521.79779341017</v>
+        <v>95311.758711911796</v>
       </c>
       <c r="O54" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653025E-2</v>
+        <v>6.2542357279826807E-2</v>
       </c>
       <c r="P54" s="8">
         <f t="shared" si="5"/>
-        <v>56803.137900818525</v>
+        <v>49593.098819320141</v>
       </c>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
@@ -6295,8 +6295,8 @@
         <v>0</v>
       </c>
       <c r="E55" s="5">
-        <f t="shared" si="9"/>
-        <v>-1516.9909873951947</v>
+        <f t="shared" si="10"/>
+        <v>-1883.1032884341075</v>
       </c>
       <c r="F55" s="5">
         <f t="shared" si="12"/>
@@ -6304,7 +6304,7 @@
       </c>
       <c r="G55" s="5">
         <f t="shared" si="14"/>
-        <v>8677.7289464463156</v>
+        <v>8424.9795596566164</v>
       </c>
       <c r="H55" s="5">
         <v>0</v>
@@ -6322,15 +6322,15 @@
       </c>
       <c r="N55" s="8">
         <f t="shared" si="6"/>
-        <v>105597.45172721252</v>
+        <v>98171.111473269179</v>
       </c>
       <c r="O55" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653053E-2</v>
+        <v>6.2542357279826821E-2</v>
       </c>
       <c r="P55" s="8">
         <f t="shared" si="5"/>
-        <v>58507.232037843081</v>
+        <v>51080.891783899737</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
@@ -6348,8 +6348,8 @@
         <v>0</v>
       </c>
       <c r="E56" s="5">
-        <f t="shared" si="9"/>
-        <v>-1562.5007170170506</v>
+        <f t="shared" si="10"/>
+        <v>-1939.5963870871308</v>
       </c>
       <c r="F56" s="5">
         <f t="shared" si="12"/>
@@ -6357,7 +6357,7 @@
       </c>
       <c r="G56" s="5">
         <f t="shared" si="14"/>
-        <v>8938.0608148397059</v>
+        <v>8677.7289464463156</v>
       </c>
       <c r="H56" s="5">
         <v>0</v>
@@ -6375,15 +6375,15 @@
       </c>
       <c r="N56" s="8">
         <f t="shared" si="6"/>
-        <v>108765.37527902891</v>
+        <v>101116.24481746728</v>
       </c>
       <c r="O56" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653067E-2</v>
+        <v>6.2542357279826835E-2</v>
       </c>
       <c r="P56" s="8">
         <f t="shared" si="5"/>
-        <v>60262.448998978376</v>
+        <v>52613.318537416737</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
@@ -6401,8 +6401,8 @@
         <v>0</v>
       </c>
       <c r="E57" s="5">
-        <f t="shared" si="9"/>
-        <v>-1609.3757385275621</v>
+        <f t="shared" si="10"/>
+        <v>-1997.7842786997448</v>
       </c>
       <c r="F57" s="5">
         <f t="shared" si="12"/>
@@ -6410,7 +6410,7 @@
       </c>
       <c r="G57" s="5">
         <f t="shared" si="14"/>
-        <v>9206.2026392848966</v>
+        <v>8938.0608148397059</v>
       </c>
       <c r="H57" s="5">
         <v>0</v>
@@ -6428,15 +6428,15 @@
       </c>
       <c r="N57" s="8">
         <f t="shared" si="6"/>
-        <v>112028.33653739968</v>
+        <v>104149.73216199118</v>
       </c>
       <c r="O57" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727652998E-2</v>
+        <v>6.2542357279826766E-2</v>
       </c>
       <c r="P57" s="8">
         <f t="shared" si="5"/>
-        <v>62070.322468947728</v>
+        <v>54191.718093539239</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
@@ -6454,8 +6454,8 @@
         <v>0</v>
       </c>
       <c r="E58" s="5">
-        <f t="shared" si="9"/>
-        <v>-1657.657010683389</v>
+        <f t="shared" si="10"/>
+        <v>-2057.7178070607374</v>
       </c>
       <c r="F58" s="5">
         <f t="shared" si="12"/>
@@ -6463,7 +6463,7 @@
       </c>
       <c r="G58" s="5">
         <f t="shared" si="14"/>
-        <v>9482.3887184634441</v>
+        <v>9206.2026392848966</v>
       </c>
       <c r="H58" s="5">
         <v>0</v>
@@ -6481,15 +6481,15 @@
       </c>
       <c r="N58" s="8">
         <f t="shared" si="6"/>
-        <v>115389.18663352184</v>
+        <v>107274.22412685108</v>
       </c>
       <c r="O58" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653095E-2</v>
+        <v>6.2542357279826863E-2</v>
       </c>
       <c r="P58" s="8">
         <f t="shared" si="5"/>
-        <v>63932.432143016165</v>
+        <v>55817.469636345413</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.2">
@@ -6507,8 +6507,8 @@
         <v>0</v>
       </c>
       <c r="E59" s="5">
-        <f t="shared" si="9"/>
-        <v>-1707.3867210038907</v>
+        <f t="shared" si="10"/>
+        <v>-2119.4493412725596</v>
       </c>
       <c r="F59" s="5">
         <f t="shared" si="12"/>
@@ -6516,7 +6516,7 @@
       </c>
       <c r="G59" s="5">
         <f t="shared" si="14"/>
-        <v>9766.8603800173478</v>
+        <v>9482.3887184634441</v>
       </c>
       <c r="H59" s="5">
         <v>0</v>
@@ -6534,15 +6534,15 @@
       </c>
       <c r="N59" s="8">
         <f t="shared" si="6"/>
-        <v>118850.86223252733</v>
+        <v>110492.45085065646</v>
       </c>
       <c r="O59" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727652998E-2</v>
+        <v>6.2542357279826766E-2</v>
       </c>
       <c r="P59" s="8">
         <f t="shared" si="5"/>
-        <v>65850.405107306651</v>
+        <v>57491.993725435779</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.2">
@@ -6560,8 +6560,8 @@
         <v>0</v>
       </c>
       <c r="E60" s="5">
-        <f t="shared" si="9"/>
-        <v>-1758.6083226340074</v>
+        <f t="shared" si="10"/>
+        <v>-2183.0328215107365</v>
       </c>
       <c r="F60" s="5">
         <f t="shared" si="12"/>
@@ -6569,7 +6569,7 @@
       </c>
       <c r="G60" s="5">
         <f t="shared" si="14"/>
-        <v>10059.866191417868</v>
+        <v>9766.8603800173478</v>
       </c>
       <c r="H60" s="5">
         <v>0</v>
@@ -6587,15 +6587,15 @@
       </c>
       <c r="N60" s="8">
         <f t="shared" si="6"/>
-        <v>122416.38809950333</v>
+        <v>113807.22437617634</v>
       </c>
       <c r="O60" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653095E-2</v>
+        <v>6.2542357279826877E-2</v>
       </c>
       <c r="P60" s="8">
         <f t="shared" si="5"/>
-        <v>67825.917260525835</v>
+        <v>59216.753537198849</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.2">
@@ -6613,8 +6613,8 @@
         <v>0</v>
       </c>
       <c r="E61" s="5">
-        <f t="shared" si="9"/>
-        <v>-1811.3665723130277</v>
+        <f t="shared" si="10"/>
+        <v>-2248.5238061560585</v>
       </c>
       <c r="F61" s="5">
         <f t="shared" si="12"/>
@@ -6622,7 +6622,7 @@
       </c>
       <c r="G61" s="5">
         <f t="shared" si="14"/>
-        <v>10361.662177160404</v>
+        <v>10059.866191417868</v>
       </c>
       <c r="H61" s="5">
         <v>0</v>
@@ -6640,15 +6640,15 @@
       </c>
       <c r="N61" s="8">
         <f t="shared" si="6"/>
-        <v>126088.87974248832</v>
+        <v>117221.44110746152</v>
       </c>
       <c r="O61" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653039E-2</v>
+        <v>6.2542357279826807E-2</v>
       </c>
       <c r="P61" s="8">
         <f t="shared" si="5"/>
-        <v>69860.694778341625</v>
+        <v>60993.256143314815</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
@@ -6666,8 +6666,8 @@
         <v>0</v>
       </c>
       <c r="E62" s="5">
-        <f t="shared" si="9"/>
-        <v>-1865.7075694824186</v>
+        <f t="shared" si="10"/>
+        <v>-2315.9795203407402</v>
       </c>
       <c r="F62" s="5">
         <f t="shared" si="12"/>
@@ -6675,7 +6675,7 @@
       </c>
       <c r="G62" s="5">
         <f t="shared" si="14"/>
-        <v>10672.512042475217</v>
+        <v>10361.662177160404</v>
       </c>
       <c r="H62" s="5">
         <v>0</v>
@@ -6693,15 +6693,15 @@
       </c>
       <c r="N62" s="8">
         <f t="shared" si="6"/>
-        <v>129871.54613476286</v>
+        <v>120738.08434068525</v>
       </c>
       <c r="O62" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727652984E-2</v>
+        <v>6.2542357279826752E-2</v>
       </c>
       <c r="P62" s="8">
         <f t="shared" si="5"/>
-        <v>71956.515621691869</v>
+        <v>62823.053827614254</v>
       </c>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
@@ -6719,8 +6719,8 @@
         <v>0</v>
       </c>
       <c r="E63" s="5">
-        <f t="shared" si="9"/>
-        <v>-1921.6787965668912</v>
+        <f t="shared" si="10"/>
+        <v>-2385.4589059509626</v>
       </c>
       <c r="F63" s="5">
         <f t="shared" si="12"/>
@@ -6728,7 +6728,7 @@
       </c>
       <c r="G63" s="5">
         <f t="shared" si="14"/>
-        <v>10992.687403749473</v>
+        <v>10672.512042475217</v>
       </c>
       <c r="H63" s="5">
         <v>0</v>
@@ -6746,15 +6746,15 @@
       </c>
       <c r="N63" s="8">
         <f t="shared" si="6"/>
-        <v>133767.69251880585</v>
+        <v>124360.22687090594</v>
       </c>
       <c r="O63" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653039E-2</v>
+        <v>6.2542357279826821E-2</v>
       </c>
       <c r="P63" s="8">
         <f t="shared" si="5"/>
-        <v>74115.211090342622</v>
+        <v>64707.745442442698</v>
       </c>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
@@ -6772,8 +6772,8 @@
         <v>0</v>
       </c>
       <c r="E64" s="5">
-        <f t="shared" si="9"/>
-        <v>-1979.329160463898</v>
+        <f t="shared" si="10"/>
+        <v>-2457.0226731294915</v>
       </c>
       <c r="F64" s="5">
         <f t="shared" si="12"/>
@@ -6781,7 +6781,7 @@
       </c>
       <c r="G64" s="5">
         <f t="shared" si="14"/>
-        <v>11322.468025861957</v>
+        <v>10992.687403749473</v>
       </c>
       <c r="H64" s="5">
         <v>0</v>
@@ -6799,15 +6799,15 @@
       </c>
       <c r="N64" s="8">
         <f t="shared" si="6"/>
-        <v>137780.72329437005</v>
+        <v>128091.03367703313</v>
       </c>
       <c r="O64" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653039E-2</v>
+        <v>6.2542357279826821E-2</v>
       </c>
       <c r="P64" s="8">
         <f t="shared" si="5"/>
-        <v>76338.667423052902</v>
+        <v>66648.977805715971</v>
       </c>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
@@ -6825,8 +6825,8 @@
         <v>0</v>
       </c>
       <c r="E65" s="5">
-        <f t="shared" si="9"/>
-        <v>-2038.709035277815</v>
+        <f t="shared" si="10"/>
+        <v>-2530.7333533233764</v>
       </c>
       <c r="F65" s="5">
         <f t="shared" si="12"/>
@@ -6834,7 +6834,7 @@
       </c>
       <c r="G65" s="5">
         <f t="shared" si="14"/>
-        <v>11662.142066637816</v>
+        <v>11322.468025861957</v>
       </c>
       <c r="H65" s="5">
         <v>0</v>
@@ -6852,15 +6852,15 @@
       </c>
       <c r="N65" s="8">
         <f t="shared" si="6"/>
-        <v>141914.14499320131</v>
+        <v>131933.76468734426</v>
       </c>
       <c r="O65" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653109E-2</v>
+        <v>6.2542357279826877E-2</v>
       </c>
       <c r="P65" s="8">
         <f t="shared" si="5"/>
-        <v>78628.827445744493</v>
+        <v>68648.447139887445</v>
       </c>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
@@ -6878,8 +6878,8 @@
         <v>0</v>
       </c>
       <c r="E66" s="5">
-        <f t="shared" si="9"/>
-        <v>-2099.8703063361495</v>
+        <f t="shared" si="10"/>
+        <v>-2606.6553539230777</v>
       </c>
       <c r="F66" s="5">
         <f t="shared" si="12"/>
@@ -6887,7 +6887,7 @@
       </c>
       <c r="G66" s="5">
         <f t="shared" si="14"/>
-        <v>12012.006328636951</v>
+        <v>11662.142066637816</v>
       </c>
       <c r="H66" s="5">
         <v>0</v>
@@ -6905,15 +6905,15 @@
       </c>
       <c r="N66" s="8">
         <f t="shared" si="6"/>
-        <v>146171.5693429971</v>
+        <v>135891.77762796436</v>
       </c>
       <c r="O66" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727652998E-2</v>
+        <v>6.2542357279826766E-2</v>
       </c>
       <c r="P66" s="8">
         <f t="shared" si="5"/>
-        <v>80987.692269116829</v>
+        <v>70707.900554084074</v>
       </c>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
@@ -6931,8 +6931,8 @@
         <v>0</v>
       </c>
       <c r="E67" s="5">
-        <f t="shared" si="9"/>
-        <v>-2162.8664155262341</v>
+        <f t="shared" si="10"/>
+        <v>-2684.8550145407698</v>
       </c>
       <c r="F67" s="5">
         <f t="shared" si="12"/>
@@ -6940,7 +6940,7 @@
       </c>
       <c r="G67" s="5">
         <f t="shared" si="14"/>
-        <v>12372.366518496061</v>
+        <v>12012.006328636951</v>
       </c>
       <c r="H67" s="5">
         <v>0</v>
@@ -6958,15 +6958,15 @@
       </c>
       <c r="N67" s="8">
         <f t="shared" si="6"/>
-        <v>150556.71642328706</v>
+        <v>139968.5309568033</v>
       </c>
       <c r="O67" s="13">
         <f t="shared" si="7"/>
-        <v>6.7273492727653011E-2</v>
+        <v>6.254235727982678E-2</v>
       </c>
       <c r="P67" s="8">
         <f t="shared" ref="P67:P71" si="16">12*(C67+D67+E67+F67+G67)+H67</f>
-        <v>83417.323037190363</v>
+        <v>72829.137570706604</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
@@ -6985,7 +6985,7 @@
       </c>
       <c r="E68" s="5">
         <f t="shared" ref="E68:E71" si="17">E67*(1+B68)</f>
-        <v>-2227.7524079920213</v>
+        <v>-2765.4006649769931</v>
       </c>
       <c r="F68" s="5">
         <f t="shared" si="12"/>
@@ -6993,7 +6993,7 @@
       </c>
       <c r="G68" s="5">
         <f t="shared" si="14"/>
-        <v>12743.537514050942</v>
+        <v>12372.366518496061</v>
       </c>
       <c r="H68" s="5">
         <v>0</v>
@@ -7011,15 +7011,15 @@
       </c>
       <c r="N68" s="8">
         <f t="shared" ref="N68:N71" si="18">M68-M67+12*(C68+D68+E68+F68+G68)+H68</f>
-        <v>155073.41791598589</v>
+        <v>144167.58688550766</v>
       </c>
       <c r="O68" s="13">
         <f t="shared" ref="O68:O71" si="19">N68/M67</f>
-        <v>6.7273492727653109E-2</v>
+        <v>6.2542357279826891E-2</v>
       </c>
       <c r="P68" s="8">
         <f t="shared" si="16"/>
-        <v>85919.842728306045</v>
+        <v>75014.011697827809</v>
       </c>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
@@ -7038,7 +7038,7 @@
       </c>
       <c r="E69" s="5">
         <f t="shared" si="17"/>
-        <v>-2294.5849802317821</v>
+        <v>-2848.3626849263028</v>
       </c>
       <c r="F69" s="5">
         <f t="shared" si="12"/>
@@ -7046,7 +7046,7 @@
       </c>
       <c r="G69" s="5">
         <f t="shared" si="14"/>
-        <v>13125.84363947247</v>
+        <v>12743.537514050942</v>
       </c>
       <c r="H69" s="5">
         <v>0</v>
@@ -7064,15 +7064,15 @@
       </c>
       <c r="N69" s="8">
         <f t="shared" si="18"/>
-        <v>159725.62045346526</v>
+        <v>148492.61449207267</v>
       </c>
       <c r="O69" s="13">
         <f t="shared" si="19"/>
-        <v>6.7273492727653011E-2</v>
+        <v>6.2542357279826793E-2</v>
       </c>
       <c r="P69" s="8">
         <f t="shared" si="16"/>
-        <v>88497.438010155223</v>
+        <v>77264.432048762639</v>
       </c>
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.2">
@@ -7091,7 +7091,7 @@
       </c>
       <c r="E70" s="5">
         <f t="shared" si="17"/>
-        <v>-2363.4225296387358</v>
+        <v>-2933.8135654740918</v>
       </c>
       <c r="F70" s="5">
         <f t="shared" si="12"/>
@@ -7099,7 +7099,7 @@
       </c>
       <c r="G70" s="5">
         <f t="shared" si="14"/>
-        <v>13519.618948656645</v>
+        <v>13125.84363947247</v>
       </c>
       <c r="H70" s="5">
         <v>0</v>
@@ -7117,15 +7117,15 @@
       </c>
       <c r="N70" s="8">
         <f t="shared" si="18"/>
-        <v>164517.38906706922</v>
+        <v>152947.39292683481</v>
       </c>
       <c r="O70" s="13">
         <f t="shared" si="19"/>
-        <v>6.7273492727653011E-2</v>
+        <v>6.254235727982678E-2</v>
       </c>
       <c r="P70" s="8">
         <f t="shared" si="16"/>
-        <v>91152.361150459896</v>
+        <v>79582.365010225505</v>
       </c>
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.2">
@@ -7144,7 +7144,7 @@
       </c>
       <c r="E71" s="5">
         <f t="shared" si="17"/>
-        <v>-2434.3252055278981</v>
+        <v>-3021.8279724383146</v>
       </c>
       <c r="F71" s="5">
         <f t="shared" si="12"/>
@@ -7152,7 +7152,7 @@
       </c>
       <c r="G71" s="5">
         <f t="shared" si="14"/>
-        <v>13925.207517116345</v>
+        <v>13519.618948656645</v>
       </c>
       <c r="H71" s="5">
         <v>0</v>
@@ -7170,15 +7170,15 @@
       </c>
       <c r="N71" s="8">
         <f t="shared" si="18"/>
-        <v>169452.91073908153</v>
+        <v>157535.81471464015</v>
       </c>
       <c r="O71" s="13">
         <f t="shared" si="19"/>
-        <v>6.7273492727653109E-2</v>
+        <v>6.2542357279826891E-2</v>
       </c>
       <c r="P71" s="8">
         <f t="shared" si="16"/>
-        <v>93886.931984973693</v>
+        <v>81969.835960532306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>